<commit_message>
update impact analysis and add a class diagram for the impacted classes
</commit_message>
<xml_diff>
--- a/Report_CR1.xlsx
+++ b/Report_CR1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>Software system:</t>
   </si>
@@ -72,12 +72,6 @@
     <t>2. Discuss how to approach</t>
   </si>
   <si>
-    <t>3. No impact to other classes</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Class Name</t>
   </si>
   <si>
@@ -96,12 +90,6 @@
     <t>1. Search for "titles" , "playlist"</t>
   </si>
   <si>
-    <t>1. Look for how other existing sorting function is used</t>
-  </si>
-  <si>
-    <t>2. The change will be limited to column sorting</t>
-  </si>
-  <si>
     <t>3.Creat the class under net.sourceforge.atunes.model.player package</t>
   </si>
   <si>
@@ -166,6 +154,21 @@
   </si>
   <si>
     <t>aTunes/src/net/sourceforge/atunes/model/player/PlayListDurationComparator.java</t>
+  </si>
+  <si>
+    <t>1. Marked the PlayListController as impacted: columClicked() method needs to be modified to add sortybyDuration, which is created in PlayListHandler class</t>
+  </si>
+  <si>
+    <t>2. Marked the PlayListTable as impacted:  columClicked() method is called by this class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Marked the PlayListHandler as impacted: a new method, sortPlaylistByDuratoin() is created in this class. </t>
+  </si>
+  <si>
+    <t>4. Marked the PlayListDurationComparator as impacted: This is a new class, which is used by PlayListHandler class</t>
+  </si>
+  <si>
+    <t>Impacted Classes</t>
   </si>
 </sst>
 </file>
@@ -251,8 +254,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -282,15 +295,25 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -304,6 +327,2598 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1625600</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>807085</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>31499</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Rounded Rectangle 25"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1625600" y="11772900"/>
+          <a:ext cx="8134985" cy="5213099"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2203763</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>160137</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>52770</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>148469</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="TextBox 26"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2203763" y="14257137"/>
+          <a:ext cx="2929007" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>PlayListDurationComparator</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4754747</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>166712</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1513712</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>155044</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="TextBox 27"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4754747" y="12168212"/>
+          <a:ext cx="1838965" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>PlayListController</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>422736</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>166712</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>445601</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>155044</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="TextBox 28"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7560136" y="12168212"/>
+          <a:ext cx="1838965" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>PlayListController</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4693506</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>166712</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1513712</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>168022</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="Rectangle 29"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4693506" y="12168212"/>
+          <a:ext cx="1900206" cy="1144310"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4693506</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>155044</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1513712</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>155044</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Straight Connector 30"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4693506" y="12537544"/>
+          <a:ext cx="1900206" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4693506</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>19002</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1513712</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>19002</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Straight Connector 31"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4693506" y="12973002"/>
+          <a:ext cx="1900206" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>361495</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>166712</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>445601</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>168022</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="Rectangle 32"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7498895" y="12168212"/>
+          <a:ext cx="1900206" cy="1144310"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>361495</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>155044</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>445601</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>155044</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Straight Connector 33"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7498895" y="12537544"/>
+          <a:ext cx="1900206" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>361495</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>19002</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>445601</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>19002</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Straight Connector 34"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7498895" y="12973002"/>
+          <a:ext cx="1900206" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2142522</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>160137</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>52770</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>161447</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="Rectangle 35"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2142522" y="14257137"/>
+          <a:ext cx="2990248" cy="1144310"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2142522</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>148469</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>52770</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>148469</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Straight Connector 36"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2142522" y="14626469"/>
+          <a:ext cx="2990248" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2142522</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>12427</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>52770</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>12427</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Straight Connector 37"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2142522" y="15061927"/>
+          <a:ext cx="2990248" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2081281</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>168090</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3981487</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>169400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="Rectangle 38"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2081281" y="12169590"/>
+          <a:ext cx="1900206" cy="1144310"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2142522</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>168090</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3777330</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>156422</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="TextBox 39"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2142522" y="12169590"/>
+          <a:ext cx="1634808" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>PlayListHandler</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2081281</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>156422</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3981487</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>156422</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Straight Connector 40"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2081281" y="12538922"/>
+          <a:ext cx="1900206" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2081281</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>20380</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3981487</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>20380</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="Straight Connector 41"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2081281" y="12974380"/>
+          <a:ext cx="1900206" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3981487</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>167367</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4693506</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>168745</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Straight Connector 42"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="39" idx="3"/>
+          <a:endCxn id="30" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3981487" y="12740367"/>
+          <a:ext cx="712019" cy="1378"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1513712</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>167367</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>361495</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>167367</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="Straight Connector 43"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="30" idx="3"/>
+          <a:endCxn id="33" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6593712" y="12740367"/>
+          <a:ext cx="905183" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3031384</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>169400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3668267</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>160137</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="45" name="Straight Connector 44"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="39" idx="2"/>
+          <a:endCxn id="27" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3031384" y="13313900"/>
+          <a:ext cx="636883" cy="943237"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2203982</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>184666</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2516888</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>172998</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="TextBox 45"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2203982" y="11805166"/>
+          <a:ext cx="312906" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>C</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>550097</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>882865</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>140732</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="TextBox 46"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7687497" y="11772900"/>
+          <a:ext cx="332768" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>U</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4913555</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>163213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>146461</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>151545</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="Rectangle 47"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4913555" y="11783713"/>
+          <a:ext cx="312906" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>C</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2356382</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>171557</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2690052</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>159889</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="TextBox 48"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2356382" y="13887557"/>
+          <a:ext cx="333670" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>N</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1625251</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>159693</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1079465</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>130523</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="TextBox 49"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705251" y="15590193"/>
+          <a:ext cx="1511614" cy="923330"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>C: Changed</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>N: New</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>U: Unchanged</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -569,10 +3184,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -605,7 +3220,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -616,13 +3231,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30">
@@ -630,46 +3245,46 @@
         <v>3</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="6"/>
       <c r="B8" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="6"/>
       <c r="B9" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="6"/>
       <c r="B10" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -762,7 +3377,7 @@
     <row r="22" spans="1:3">
       <c r="A22" s="6"/>
       <c r="B22" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -770,7 +3385,7 @@
         <v>5</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -788,27 +3403,27 @@
         <v>6</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="B28" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="B29" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="B30" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="B31" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -816,91 +3431,94 @@
         <v>7</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="B37" s="2" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="B38" s="2" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="B39" s="5"/>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="5" t="s">
+      <c r="B39" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="B42" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="B43" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
       <c r="B44" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="B45" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="B46" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="5" t="s">
-        <v>9</v>
-      </c>
       <c r="B47" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="B48" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="B49" s="2" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:2">
+      <c r="A50" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="B50" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="B51" s="5"/>
+      <c r="B51" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="B52" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="4" t="s">
+      <c r="B53" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="B54" s="5"/>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="6"/>
+      <c r="B56" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>